<commit_message>
Made correlation graphs for relative abundance (absolute abundances don't make a lot of sence)
</commit_message>
<xml_diff>
--- a/Data/Results/Important_taxa_with_tax.xlsx
+++ b/Data/Results/Important_taxa_with_tax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqoshopi\Dropbox\Olga Shopina\Amplicon\Networks\Data\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF2A9E-5845-41B0-B5A3-436B745F0B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B917D-B846-479D-8BF4-89B4E119977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="several_methods" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">classification!$A$1:$D$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">several_groups!$A$1:$D$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">several_methods!$A$1:$C$71</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="254">
   <si>
     <t>OTU</t>
   </si>
@@ -779,6 +780,15 @@
   </si>
   <si>
     <t>k__Fungi;p__Ascomycota;c__Sordariomycetes;o__Sordariales;f__Lasiosphaeriaceae;g__unidentified;s__unidentified</t>
+  </si>
+  <si>
+    <t>important_pH</t>
+  </si>
+  <si>
+    <t>Important_pH</t>
+  </si>
+  <si>
+    <t>pH 6; 6,5</t>
   </si>
 </sst>
 </file>
@@ -831,7 +841,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1165,20 +1186,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>252</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1354,7 +1378,7 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>253</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -1362,610 +1386,607 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
         <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
         <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B65" t="s">
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>146</v>
-      </c>
-      <c r="B72" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C71" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C71">
+      <sortCondition ref="A1:A71"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1976,7 +1997,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:D33"/>
+      <selection sqref="A1:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2465,8 +2486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2E6AC8-2D91-44A6-9A1B-3EF158BC20F9}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2480,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Paul added occurence matrix as an example
</commit_message>
<xml_diff>
--- a/Data/Results/Important_taxa_with_tax.xlsx
+++ b/Data/Results/Important_taxa_with_tax.xlsx
@@ -8,26 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqoshopi\Dropbox\Olga Shopina\Amplicon\Networks\Data\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B917D-B846-479D-8BF4-89B4E119977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D08CA60-0081-4920-A63F-E4ED6F189112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="several_methods" sheetId="1" r:id="rId1"/>
     <sheet name="several_groups" sheetId="2" r:id="rId2"/>
     <sheet name="classification" sheetId="3" r:id="rId3"/>
+    <sheet name="Paul_example" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">classification!$A$1:$D$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">several_groups!$A$1:$D$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">several_methods!$A$1:$C$71</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="262">
   <si>
     <t>OTU</t>
   </si>
@@ -789,6 +803,30 @@
   </si>
   <si>
     <t>pH 6; 6,5</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>pH4</t>
+  </si>
+  <si>
+    <t>pH4.5</t>
+  </si>
+  <si>
+    <t>pH5</t>
+  </si>
+  <si>
+    <t>pH5.5</t>
+  </si>
+  <si>
+    <t>pH6</t>
+  </si>
+  <si>
+    <t>pH6.5</t>
+  </si>
+  <si>
+    <t>pH7</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +2035,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D33"/>
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3554,4 +3592,380 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DD6BB7-FE3A-4130-95B6-1E30D5EC25AB}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I22">
+    <sortCondition ref="I2:I22"/>
+  </sortState>
+  <conditionalFormatting sqref="B2:H12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>